<commit_message>
Updated the WVD CAF Guidance document
</commit_message>
<xml_diff>
--- a/Technical Enablement/WVD CAF Project Task List.xlsx
+++ b/Technical Enablement/WVD CAF Project Task List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Github\CAF\WVD_CAF_SolutionFactory\WVD CAF Toolkit\Project Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft.sharepoint.com/teams/CAFEnablementKitDevelopment/Shared Documents/General/CAF WVD - Partner Enablement Toolkit/CAF WVD - Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072585B1-A290-4121-B1EB-B08C8DF465CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{4A6183F2-2C80-44A8-AB5E-8FEA1CACE5C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{86516D7A-6B50-4D08-AFEC-D0716CE80CFF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{86516D7A-6B50-4D08-AFEC-D0716CE80CFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,14 +31,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -276,7 +268,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Microsoft applications</t>
+      <t>Microsoft applications like office apps</t>
     </r>
   </si>
   <si>
@@ -322,7 +314,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Custom applications</t>
+      <t>Custom applications like customer business apps</t>
     </r>
   </si>
   <si>
@@ -391,7 +383,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Marketplace images</t>
+      <t>Marketplace images like predefined Azure Gallery Images</t>
     </r>
   </si>
   <si>
@@ -414,7 +406,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Custom images</t>
+      <t xml:space="preserve">Create Custom images </t>
     </r>
   </si>
   <si>
@@ -558,6 +550,29 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t>Create and configure host pools and session hosts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t>Validate Windows Virtual Desktop deployment</t>
     </r>
   </si>
@@ -565,7 +580,7 @@
     <t>Milestone 3 – Readiness - Setup landing zone</t>
   </si>
   <si>
-    <t xml:space="preserve">These items are addressed as needed and might have impact to timeline. These items will be addressed as mutually agreed by customer and partner. </t>
+    <t xml:space="preserve">During the Readinesss phase, these items will be addressed as mutually agreed by customer and partner </t>
   </si>
   <si>
     <r>
@@ -633,7 +648,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Azure Bastion</t>
+      <t>Azure Bastion Configuration to access azure virtual machine</t>
     </r>
   </si>
   <si>
@@ -932,7 +947,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Azure Sentinel</t>
+      <t>Azure Sentinel intelligent security analytics</t>
     </r>
   </si>
   <si>
@@ -1121,6 +1136,29 @@
   </si>
   <si>
     <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Business Continuity &amp; Disaster Recovery (BCDR)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>o</t>
     </r>
     <r>
@@ -1139,7 +1177,25 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Azure Backup </t>
+      <t>Perform</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Azure Site Recovery</t>
     </r>
   </si>
   <si>
@@ -1162,7 +1218,30 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Business Continuity &amp; Disaster Recovery (BCDR)</t>
+      <t>Resilient File Servers (RFS)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Windows Virtual Desktop (WVD)</t>
     </r>
   </si>
   <si>
@@ -1173,8 +1252,8 @@
       <rPr>
         <sz val="7"/>
         <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   </t>
     </r>
@@ -1185,99 +1264,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Azure Site Recovery</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Resilient File Servers (RFS)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Azure Files | Azure File Sync</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Windows Virtual Desktop (WVD)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Domain Prep</t>
+      <t>Domain Preparation</t>
     </r>
   </si>
   <si>
@@ -1662,35 +1649,48 @@
   </si>
   <si>
     <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Create and configure host pools and session hosts</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Configure Azure Backup </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sync with Azure Files | Azure File Sync</t>
     </r>
   </si>
 </sst>
@@ -1698,7 +1698,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1776,8 +1776,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1814,6 +1820,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1842,7 +1854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1889,6 +1901,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="13"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="9"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2206,21 +2234,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9838602B-A6A1-46EE-9823-4E2F494AFEEF}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="158" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -2231,7 +2259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.899999999999999" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>205000</v>
       </c>
@@ -2242,7 +2270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>205001</v>
       </c>
@@ -2253,7 +2281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>205002</v>
       </c>
@@ -2264,7 +2292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>205003</v>
       </c>
@@ -2275,7 +2303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>205004</v>
       </c>
@@ -2286,7 +2314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>205005</v>
       </c>
@@ -2297,7 +2325,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>205006</v>
       </c>
@@ -2308,7 +2336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>205007</v>
       </c>
@@ -2319,7 +2347,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>205008</v>
       </c>
@@ -2330,7 +2358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>205009</v>
       </c>
@@ -2341,18 +2369,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>205010</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>205011</v>
       </c>
@@ -2363,18 +2391,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>205012</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>205013</v>
       </c>
@@ -2385,7 +2413,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>205014</v>
       </c>
@@ -2396,18 +2424,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>205015</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>205016</v>
       </c>
@@ -2418,7 +2446,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>205017</v>
       </c>
@@ -2429,7 +2457,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>205018</v>
       </c>
@@ -2440,7 +2468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>205020</v>
       </c>
@@ -2451,7 +2479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>205021</v>
       </c>
@@ -2462,7 +2490,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16.899999999999999" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>205029</v>
       </c>
@@ -2473,7 +2501,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>205030</v>
       </c>
@@ -2484,7 +2512,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>205031</v>
       </c>
@@ -2495,7 +2523,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>205032</v>
       </c>
@@ -2503,10 +2531,10 @@
         <v>7</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>205033</v>
       </c>
@@ -2514,10 +2542,10 @@
         <v>7</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="16.899999999999999" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>205038</v>
       </c>
@@ -2525,10 +2553,10 @@
         <v>3</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>205039</v>
       </c>
@@ -2536,10 +2564,10 @@
         <v>5</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>205040</v>
       </c>
@@ -2547,10 +2575,10 @@
         <v>7</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>205041</v>
       </c>
@@ -2558,32 +2586,32 @@
         <v>7</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>205042</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" s="12">
+      <c r="C33" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="17">
         <v>205043</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C34" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>205044</v>
       </c>
@@ -2591,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>205045</v>
       </c>
@@ -2602,10 +2630,10 @@
         <v>7</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>205046</v>
       </c>
@@ -2613,10 +2641,10 @@
         <v>10</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>205047</v>
       </c>
@@ -2624,10 +2652,10 @@
         <v>10</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
         <v>205048</v>
       </c>
@@ -2635,10 +2663,10 @@
         <v>7</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="12">
         <v>205049</v>
       </c>
@@ -2646,10 +2674,10 @@
         <v>10</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="12">
         <v>205050</v>
       </c>
@@ -2657,10 +2685,10 @@
         <v>10</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
         <v>205051</v>
       </c>
@@ -2668,10 +2696,10 @@
         <v>10</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
         <v>205052</v>
       </c>
@@ -2679,10 +2707,10 @@
         <v>7</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="12">
         <v>205053</v>
       </c>
@@ -2690,10 +2718,10 @@
         <v>10</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="12">
         <v>205054</v>
       </c>
@@ -2701,10 +2729,10 @@
         <v>7</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="12">
         <v>205055</v>
       </c>
@@ -2712,10 +2740,10 @@
         <v>10</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="12">
         <v>205056</v>
       </c>
@@ -2723,10 +2751,10 @@
         <v>10</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="12">
         <v>205057</v>
       </c>
@@ -2734,10 +2762,10 @@
         <v>10</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="12">
         <v>205058</v>
       </c>
@@ -2745,10 +2773,10 @@
         <v>10</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="12">
         <v>205059</v>
       </c>
@@ -2756,10 +2784,10 @@
         <v>7</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="12">
         <v>205060</v>
       </c>
@@ -2767,10 +2795,10 @@
         <v>10</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="12">
         <v>205061</v>
       </c>
@@ -2778,10 +2806,10 @@
         <v>10</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="12">
         <v>205062</v>
       </c>
@@ -2789,10 +2817,10 @@
         <v>10</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="12">
         <v>205063</v>
       </c>
@@ -2800,10 +2828,10 @@
         <v>7</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="12">
         <v>205064</v>
       </c>
@@ -2811,10 +2839,10 @@
         <v>10</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="12">
         <v>205065</v>
       </c>
@@ -2825,7 +2853,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="12">
         <v>205066</v>
       </c>
@@ -2836,7 +2864,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="12">
         <v>205067</v>
       </c>
@@ -2847,7 +2875,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="12">
         <v>205068</v>
       </c>
@@ -2855,10 +2883,10 @@
         <v>10</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="12">
         <v>205069</v>
       </c>
@@ -2866,21 +2894,21 @@
         <v>7</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="12">
         <v>205070</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C61" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="12">
         <v>205071</v>
       </c>
@@ -2888,10 +2916,10 @@
         <v>10</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="12">
         <v>205072</v>
       </c>
@@ -2899,10 +2927,10 @@
         <v>10</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="12">
         <v>205073</v>
       </c>
@@ -2910,10 +2938,10 @@
         <v>10</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="12">
         <v>205074</v>
       </c>
@@ -2921,10 +2949,10 @@
         <v>10</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="12">
         <v>205075</v>
       </c>
@@ -2932,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16.899999999999999" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A67" s="12">
         <v>205078</v>
       </c>
@@ -2943,10 +2971,10 @@
         <v>3</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="12">
         <v>205079</v>
       </c>
@@ -2954,10 +2982,10 @@
         <v>5</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="12">
         <v>205080</v>
       </c>
@@ -2965,10 +2993,10 @@
         <v>7</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="12">
         <v>205081</v>
       </c>
@@ -2976,10 +3004,10 @@
         <v>10</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="12">
         <v>205082</v>
       </c>
@@ -2987,10 +3015,10 @@
         <v>10</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="16.899999999999999" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A72" s="12">
         <v>205087</v>
       </c>
@@ -2998,10 +3026,10 @@
         <v>3</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="12">
         <v>205088</v>
       </c>
@@ -3009,10 +3037,10 @@
         <v>5</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="12">
         <v>205089</v>
       </c>
@@ -3023,7 +3051,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="12">
         <v>205090</v>
       </c>
@@ -3031,10 +3059,10 @@
         <v>10</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="12">
         <v>205091</v>
       </c>
@@ -3042,10 +3070,10 @@
         <v>10</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="16.899999999999999" x14ac:dyDescent="0.45">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A77" s="12">
         <v>205097</v>
       </c>
@@ -3053,10 +3081,10 @@
         <v>3</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="12">
         <v>205098</v>
       </c>
@@ -3064,10 +3092,10 @@
         <v>5</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="12">
         <v>205099</v>
       </c>
@@ -3075,10 +3103,10 @@
         <v>10</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="12">
         <v>205100</v>
       </c>
@@ -3086,10 +3114,10 @@
         <v>10</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="12">
         <v>205101</v>
       </c>
@@ -3097,10 +3125,10 @@
         <v>10</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="12">
         <v>205102</v>
       </c>
@@ -3108,7 +3136,7 @@
         <v>10</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3118,6 +3146,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3126,7 +3160,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100663FA498C683E94696A9F9E86390AA5F" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="91abef37ac3c4a289a82c715eca548e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="24ce65f2-f4ee-4734-b023-07c740501d91" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="93780468c6c271b3523095b5e6847ddd" ns2:_="">
     <xsd:import namespace="24ce65f2-f4ee-4734-b023-07c740501d91"/>
@@ -3278,13 +3312,23 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEA32119-275C-4348-888C-32A7B8CE6DF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="24ce65f2-f4ee-4734-b023-07c740501d91"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B72C57D-EF25-4D42-8981-9E37446D1C21}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -3292,7 +3336,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{000F88EE-B2C4-49EA-A434-1EB421CE5FA0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3308,13 +3352,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEA32119-275C-4348-888C-32A7B8CE6DF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>